<commit_message>
More cleaning up and niceness
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/orders/OrderFiles/Hillcrest Foods/Hillcrest Foods _ BAKERY 02032025.xlsx
+++ b/WorkBot/main/backend/orders/OrderFiles/Hillcrest Foods/Hillcrest Foods _ BAKERY 02032025.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -498,7 +498,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>$504.93</t>
+          <t>$1,178.17</t>
         </is>
       </c>
     </row>
@@ -704,7 +704,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -714,7 +714,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>$1,689.00</t>
+          <t>$1,013.40</t>
         </is>
       </c>
     </row>

</xml_diff>